<commit_message>
created separate directory for resources
</commit_message>
<xml_diff>
--- a/ddf--schema.xlsx
+++ b/ddf--schema.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kacper\Desktop\Voting Sys Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kacper\Desktop\votograph\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="ddf--schema" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ddf--schema'!$A$1:$Q$1</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -7747,8 +7750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q550"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23552,6 +23555,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Q1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>